<commit_message>
Correcciones y casos de prueba
Se actualiza el codigo fuente con sus métodos de validación.

Se agregan los casos de prueba. Solo faltan hacer andar los casos de
prueba 8, 9 y 10.

Se actualiza el Excel de correspondiente.
</commit_message>
<xml_diff>
--- a/documentacion/Casos de prueba.xlsx
+++ b/documentacion/Casos de prueba.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laboratorios\Desktop\Grupo 9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Documents\GitHub\Triangulo\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14325" windowHeight="6225"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Nº de Caso</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Valor Obtenido</t>
   </si>
   <si>
-    <t>1,2,3</t>
-  </si>
-  <si>
     <t>Escaleno</t>
   </si>
   <si>
@@ -94,6 +91,12 @@
   </si>
   <si>
     <t>Los lados del triangulo debe ser mayor a 0</t>
+  </si>
+  <si>
+    <t>7,5,3</t>
+  </si>
+  <si>
+    <t>La suma de los primeros dos lados es menor al tercero</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,6 +437,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -653,7 +668,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -665,7 +680,10 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -992,7 +1010,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,13 +1039,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1035,13 +1053,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1049,13 +1067,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1063,13 +1081,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1077,13 +1095,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,13 +1109,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1105,55 +1123,55 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>16</v>
+      <c r="D9" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
+      <c r="D10" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>18</v>
+      <c r="C11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,13 +1179,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,13 +1193,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,10 +1210,10 @@
         <v>1.2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>